<commit_message>
commit noticias eexcel changes
</commit_message>
<xml_diff>
--- a/Analisis Info No estructurada/noticias_completed.xlsx
+++ b/Analisis Info No estructurada/noticias_completed.xlsx
@@ -55,13 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,57 +491,171 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Iberdrola.</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Social</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve"> People Centric</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Promover los derechos de las mujeres.</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve"> No</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t xml:space="preserve"> No.</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Personas interesadas en deporte femenino.</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Ocio y Medioambiental.</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t xml:space="preserve"> ODS 5: Igualdad de Género.</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Las jugadoras de la selección española femenina.</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Noticia</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iberdrola.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Social.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> People Centric.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Impulsar la oferta cultural en el mundo rural.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> No.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> No.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Personas del mundo rural.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Desarrollo Comunitario, Medioambiental.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ODS 11: Ciudades y Comunidades Sostenibles.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Vecinos, nios, mayores, veraneantes y todos los habitantes del mundo rural.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Noticia</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Engie.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Medioambiental.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Planet Positive.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Descarbonizar la industria y mejorar la dependencia energética del exterior.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ENAGS Renovable, Fivet Hydrogen Pontegadea, Navantia.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sí, hay otras empresas que colaboran con la empresa principal. Las empresas son: Ardian (privada), Fivet Hydrogen Pontegadea (privada), Navantia (pública) y ENAGS (privada).</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La industria de la región de Murcia.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Medioambiente.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ODS 7.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La región de Murcia, Repsol, ENAGS Renovable, Engie, la industria del Valle de Escombreras y la Asociación Sectorial del Hidrógeno Verde en la Región de Murcia.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Noticia</t>
         </is>

</xml_diff>